<commit_message>
Demarrage de la doc technique
</commit_message>
<xml_diff>
--- a/firmware/TouchGFX/assets/texts/texts.xlsx
+++ b/firmware/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="78">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t xml:space="preserve">Retour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,a-z,A-Z</t>
   </si>
 </sst>
 </file>
@@ -1492,7 +1495,7 @@
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="J4" t="s">
         <v>53</v>
@@ -1865,23 +1868,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13">
-      <c r="B13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" t="s">
-        <v>76</v>
-      </c>
-    </row>
+    <row r="13"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
mise a jour de l'IHM + docs
</commit_message>
<xml_diff>
--- a/firmware/TouchGFX/assets/texts/texts.xlsx
+++ b/firmware/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="79">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t xml:space="preserve">0-9,a-z,A-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARM-ADA</t>
   </si>
 </sst>
 </file>
@@ -1746,7 +1749,7 @@
         <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6">

</xml_diff>